<commit_message>
fix id error variable in set_gain
</commit_message>
<xml_diff>
--- a/MyTargetlist.xlsx
+++ b/MyTargetlist.xlsx
@@ -351,7 +351,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -691,7 +691,7 @@
         <v>20</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>100</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>